<commit_message>
afc bournemouth link change
</commit_message>
<xml_diff>
--- a/May_2024/may_2024.xlsx
+++ b/May_2024/may_2024.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27720"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A60C21FC-6EFD-4A69-B103-1F9740C64555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A050E6DD-9F09-47BA-B6DC-78F57AE58B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4677,7 +4677,7 @@
     <t>https://www.instagram.com/afcb</t>
   </si>
   <si>
-    <t>https://www.facebook.com/afcbournemouth/</t>
+    <t>https://www.facebook.com/afcb/</t>
   </si>
   <si>
     <t>https://www.tiktok.com/@afcb</t>
@@ -5985,8 +5985,8 @@
   <dimension ref="A1:M305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G64" sqref="G64"/>
+      <pane ySplit="1" topLeftCell="A252" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D257" sqref="D257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16438,6 +16438,9 @@
       <c r="C256">
         <v>937573</v>
       </c>
+      <c r="D256">
+        <v>810000</v>
+      </c>
       <c r="E256">
         <v>1300000</v>
       </c>
@@ -16447,7 +16450,7 @@
       <c r="G256" t="s">
         <v>1547</v>
       </c>
-      <c r="H256" t="s">
+      <c r="H256" s="3" t="s">
         <v>1548</v>
       </c>
       <c r="I256" t="s">
@@ -18490,6 +18493,7 @@
     <hyperlink ref="G82" r:id="rId11" xr:uid="{11508DAA-6A19-4973-BE00-0BAEAA98CC1B}"/>
     <hyperlink ref="J71" r:id="rId12" xr:uid="{C6BC986A-3A52-425D-B265-12DA1AA8B013}"/>
     <hyperlink ref="G64" r:id="rId13" xr:uid="{F8CB8911-E244-456C-A459-520D6176FD02}"/>
+    <hyperlink ref="H256" r:id="rId14" xr:uid="{CAE56DB1-21FA-4058-9C07-0F568AFADF8B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>